<commit_message>
docs: Upload latest version of MS Projects for S2 & S3
</commit_message>
<xml_diff>
--- a/Docs/Iteración 2/MS Project/Seguimiento de Costes del Sprint 2.xlsx
+++ b/Docs/Iteración 2/MS Project/Seguimiento de Costes del Sprint 2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\angel\Desktop\Universidad\4º AÑO\PGPI-G1.15\Docs\Iteración 2\MS Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{15331587-BBAF-4245-BF8C-5D1DCFA6D621}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{20F1F11F-6207-4B17-B10F-3BD9B2BBF815}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{B49EC062-8518-4045-B0E0-5C5C91D7AF14}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{12B9CE91-9536-470B-A2C0-ABF75DA15D70}"/>
   </bookViews>
   <sheets>
     <sheet name="Gráfico1" sheetId="2" r:id="rId1"/>
@@ -36,9 +36,9 @@
 
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
 <connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16">
-  <connection id="1" xr16:uid="{5DEB7CC1-032A-44D8-BEB2-345A1DF3C029}" sourceFile="D:\Documents and Settings\PKMACCT\My Documents\Assignment Usage.cub" keepAlive="1" name="Assignment Usage" type="5" refreshedVersion="8">
+  <connection id="1" xr16:uid="{0F46DFFE-B1FB-4A2C-92E3-38B1621BCC46}" sourceFile="D:\Documents and Settings\PKMACCT\My Documents\Assignment Usage.cub" keepAlive="1" name="Assignment Usage" type="5" refreshedVersion="8">
     <dbPr connection="Provider=MSOLAP.2;Persist Security Info=True;Data Source=D:\Documents and Settings\PKMACCT\My Documents\Assignment Usage.cub;Client Cache Size=25;Auto Synch Period=10000" command="ProjectReport" commandType="1"/>
-    <olapPr local="1" localConnection="Provider=MSOLAP.8;Persist Security Info=True;Data Source=C:\Users\angel\AppData\Local\Temp\VisualReportsTemporaryData\{dec4cfae-b3ae-ef11-905f-c38c60dbbcf3}\AssignmentTP.cub;MDX Compatibility=1;Safety Options=2;MDX Missing Member Mode=Error;Update Isolation Level=2" rowDrillCount="1000" serverFill="0" serverNumberFormat="0" serverFont="0" serverFontColor="0"/>
+    <olapPr local="1" localConnection="Provider=MSOLAP.8;Persist Security Info=True;Data Source=C:\Users\angel\AppData\Local\Temp\VisualReportsTemporaryData\{9bb86c37-3aaf-ef11-905f-c38c60dbbcf3}\AssignmentTP.cub;MDX Compatibility=1;Safety Options=2;MDX Missing Member Mode=Error;Update Isolation Level=2" rowDrillCount="1000" serverFill="0" serverNumberFormat="0" serverFont="0" serverFontColor="0"/>
   </connection>
 </connections>
 </file>
@@ -556,10 +556,10 @@
                   <c:v>849.6790123456791</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>481.56774193548387</c:v>
+                  <c:v>481.56774193548392</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>360.38637499999999</c:v>
+                  <c:v>437.9489857526882</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>13</c:v>
@@ -575,7 +575,7 @@
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-2380-4CB3-BC11-72D81FCF509C}"/>
+              <c16:uniqueId val="{00000000-03FA-4088-B614-CA9029B60292}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -694,7 +694,7 @@
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000005-2380-4CB3-BC11-72D81FCF509C}"/>
+              <c16:uniqueId val="{00000001-03FA-4088-B614-CA9029B60292}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -707,11 +707,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="841491359"/>
+        <c:axId val="627522512"/>
         <c:axId val="1"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="841491359"/>
+        <c:axId val="627522512"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -780,7 +780,7 @@
             <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="841491359"/>
+        <c:crossAx val="627522512"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -808,7 +808,7 @@
 </file>
 
 <file path=xl/chartsheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{91631F9B-EA00-4AF9-9F64-6E7C442BCCA2}">
+<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{BA08BA21-5E09-4A7C-BBAA-CC3596B485F4}">
   <sheetPr/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" workbookViewId="0"/>
@@ -830,7 +830,7 @@
         <xdr:cNvPr id="2" name="Gráfico 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{60049A60-2275-0B67-FCDB-20D9BB9172B0}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7EB06E47-A28E-A0D2-95BD-D86D5FEDF7FF}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -854,7 +854,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" saveData="0" refreshedBy="Angel Garcia" refreshedDate="45626.069860995369" createdVersion="8" refreshedVersion="8" recordCount="0" supportSubquery="1" supportAdvancedDrill="1" xr:uid="{E81F33E5-2C6C-4E70-AE36-361BF5632171}">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" saveData="0" refreshedBy="Angel Garcia" refreshedDate="45626.738822222222" createdVersion="8" refreshedVersion="8" recordCount="0" supportSubquery="1" supportAdvancedDrill="1" xr:uid="{331101DB-D066-4CC7-8176-2F1ED7D32330}">
   <cacheSource type="external" connectionId="1"/>
   <cacheFields count="48">
     <cacheField name="[Measures].[Costo real]" caption="Costo real" numFmtId="0" hierarchy="68"/>
@@ -1153,7 +1153,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{CB670AB8-544E-482C-94F5-4DFA5C67A48B}" name="PivotTable1" cacheId="19" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Datos" grandTotalCaption="Total general" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" subtotalHiddenItems="1" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" compactData="0" gridDropZones="1" chartFormat="1" fieldListSortAscending="1">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{C979265D-1934-42D6-96A6-EAC80B165C3A}" name="PivotTable1" cacheId="19" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Datos" grandTotalCaption="Total general" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" subtotalHiddenItems="1" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" compactData="0" gridDropZones="1" chartFormat="1" fieldListSortAscending="1">
   <location ref="A3:E19" firstHeaderRow="1" firstDataRow="2" firstDataCol="3" rowPageCount="1" colPageCount="1"/>
   <pivotFields count="48">
     <pivotField name="Costo real" dataField="1" compact="0" outline="0" subtotalTop="0" showAll="0" includeNewItemsInFilter="1"/>
@@ -1751,7 +1751,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{10713C53-F6D9-4324-B324-602F68F9FDD4}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB51ACAF-F973-4A02-AABE-33E3ABEA30B0}">
   <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1908,7 +1908,7 @@
         <v>18</v>
       </c>
       <c r="D12" s="10">
-        <v>481.56774193548387</v>
+        <v>481.56774193548392</v>
       </c>
       <c r="E12" s="11">
         <v>1113.5677419354838</v>
@@ -1921,7 +1921,7 @@
         <v>19</v>
       </c>
       <c r="D13" s="10">
-        <v>360.38637499999999</v>
+        <v>437.9489857526882</v>
       </c>
       <c r="E13" s="11">
         <v>1951.5677419354838</v>
@@ -1973,7 +1973,7 @@
       </c>
       <c r="C17" s="2"/>
       <c r="D17" s="6">
-        <v>2882.4896131186906</v>
+        <v>2960.0522238713788</v>
       </c>
       <c r="E17" s="7">
         <v>10142.274545454544</v>
@@ -1986,7 +1986,7 @@
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
       <c r="D18" s="6">
-        <v>2886.3241169354847</v>
+        <v>2963.8867276881729</v>
       </c>
       <c r="E18" s="7">
         <v>10146.079999999998</v>
@@ -1999,7 +1999,7 @@
       <c r="B19" s="13"/>
       <c r="C19" s="13"/>
       <c r="D19" s="14">
-        <v>2886.3241169354847</v>
+        <v>2963.8867276881729</v>
       </c>
       <c r="E19" s="15">
         <v>10146.079999999998</v>

</xml_diff>